<commit_message>
Change sheet name in the downloadable file
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapto\OneDrive\Pulpit\Social-Media\Social-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3973EA-7899-43E7-9113-3B524124C0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E204A30-3297-4236-95FD-E80434B121CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TR360" sheetId="1" r:id="rId1"/>
+    <sheet name="Social Media" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>